<commit_message>
feature: updating the java fdoc
</commit_message>
<xml_diff>
--- a/data/branch_list_updated.xlsx
+++ b/data/branch_list_updated.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2023S2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CABAEA2-29CC-4B6E-85CA-8D634B514C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{1CABAEA2-29CC-4B6E-85CA-8D634B514C40}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}" yWindow="-108" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="staff" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$A$88</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">staff!$1:$1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -65,12 +61,19 @@
   </si>
   <si>
     <t>Staff Quota</t>
+  </si>
+  <si>
+    <t>NUS</t>
+  </si>
+  <si>
+    <t>kentridge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,26 +144,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -177,10 +180,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -215,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -267,7 +270,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -378,21 +381,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -409,7 +412,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -461,318 +464,76 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:C87"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>8</v>
+      <c r="C3" t="n">
+        <v>8.0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>15</v>
+      <c r="C4" t="n">
+        <v>15.0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>11</v>
+      <c r="C5" t="n">
+        <v>11.0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="3"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="8"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="2"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="2"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="2"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2"/>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>15.0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>